<commit_message>
Big chances in the project
</commit_message>
<xml_diff>
--- a/Uitvoering Documenten/85866_PhilipKlok_ExPVB25604_Strokenplanning_Pog1.xlsx
+++ b/Uitvoering Documenten/85866_PhilipKlok_ExPVB25604_Strokenplanning_Pog1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/e-expansionict/Documents/PKstage/Examen Philip Klok/Examen_E-Expansion/Uitvoering Documenten/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9257D8-78A3-084F-9333-2C915F48E5C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83AB674B-3E2A-2B4F-BEB2-4AA9E9D2EA0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5700" yWindow="10060" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26100" yWindow="500" windowWidth="18700" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="4" r:id="rId1"/>
@@ -215,7 +215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Project:</t>
   </si>
@@ -313,13 +313,25 @@
     <t>Examenportfolio uitwerken</t>
   </si>
   <si>
-    <t xml:space="preserve">Multi-Step form uitwerken </t>
-  </si>
-  <si>
     <t>Multi-Step form informatie verzamelen</t>
   </si>
   <si>
     <t>Multi-Step form gereed</t>
+  </si>
+  <si>
+    <t>Multi-Step form start</t>
+  </si>
+  <si>
+    <t>Multi-Step form opmaak stap 1 en stap 2</t>
+  </si>
+  <si>
+    <t>Multi-Step form Knoppen functioneel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi-Step form Resultaat geprogrammeerd </t>
+  </si>
+  <si>
+    <t>Multi-Step form errors + comments</t>
   </si>
 </sst>
 </file>
@@ -1474,10 +1486,10 @@
   <dimension ref="A1:AG107"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="5" ySplit="7" topLeftCell="F8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="7" topLeftCell="L19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C5" sqref="C5"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
-      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomRight" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2620,7 +2632,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="22"/>
       <c r="D15" s="64">
@@ -2721,11 +2733,11 @@
         <v>9</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C16" s="21"/>
       <c r="D16" s="64">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="E16" s="26"/>
       <c r="F16" s="30">
@@ -2738,7 +2750,7 @@
       </c>
       <c r="H16" s="30">
         <f>IF($D16-SUM($E16:G16)&gt;H$5-SUM(H$7:H15),H$5-SUM(H$7:H15),$D16-SUM($E16:G16))</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I16" s="30">
         <f>IF($D16-SUM($E16:H16)&gt;I$5-SUM(I$7:I15),I$5-SUM(I$7:I15),$D16-SUM($E16:H16))</f>
@@ -2752,19 +2764,19 @@
       <c r="L16" s="30"/>
       <c r="M16" s="30">
         <f>IF($D16-SUM($E16:L16)&gt;M$5-SUM(M$7:M15),M$5-SUM(M$7:M15),$D16-SUM($E16:L16))</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="N16" s="30">
         <f>IF($D16-SUM($E16:M16)&gt;N$5-SUM(N$7:N15),N$5-SUM(N$7:N15),$D16-SUM($E16:M16))</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="O16" s="30">
         <f>IF($D16-SUM($E16:N16)&gt;O$5-SUM(O$7:O15),O$5-SUM(O$7:O15),$D16-SUM($E16:N16))</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="P16" s="30">
         <f>IF($D16-SUM($E16:O16)&gt;P$5-SUM(P$7:P15),P$5-SUM(P$7:P15),$D16-SUM($E16:O16))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q16" s="30">
         <f>IF($D16-SUM($E16:P16)&gt;Q$5-SUM(Q$7:Q15),Q$5-SUM(Q$7:Q15),$D16-SUM($E16:P16))</f>
@@ -2822,11 +2834,11 @@
         <v>10</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C17" s="21"/>
       <c r="D17" s="64">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E17" s="26"/>
       <c r="F17" s="30">
@@ -2839,7 +2851,7 @@
       </c>
       <c r="H17" s="30">
         <f>IF($D17-SUM($E17:G17)&gt;H$5-SUM(H$7:H16),H$5-SUM(H$7:H16),$D17-SUM($E17:G17))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I17" s="30">
         <f>IF($D17-SUM($E17:H17)&gt;I$5-SUM(I$7:I16),I$5-SUM(I$7:I16),$D17-SUM($E17:H17))</f>
@@ -2853,7 +2865,7 @@
       <c r="L17" s="30"/>
       <c r="M17" s="30">
         <f>IF($D17-SUM($E17:L17)&gt;M$5-SUM(M$7:M16),M$5-SUM(M$7:M16),$D17-SUM($E17:L17))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N17" s="30">
         <f>IF($D17-SUM($E17:M17)&gt;N$5-SUM(N$7:N16),N$5-SUM(N$7:N16),$D17-SUM($E17:M17))</f>
@@ -2865,7 +2877,7 @@
       </c>
       <c r="P17" s="30">
         <f>IF($D17-SUM($E17:O17)&gt;P$5-SUM(P$7:P16),P$5-SUM(P$7:P16),$D17-SUM($E17:O17))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q17" s="30">
         <f>IF($D17-SUM($E17:P17)&gt;Q$5-SUM(Q$7:Q16),Q$5-SUM(Q$7:Q16),$D17-SUM($E17:P17))</f>
@@ -2923,11 +2935,11 @@
         <v>11</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C18" s="22"/>
       <c r="D18" s="64">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E18" s="26"/>
       <c r="F18" s="30">
@@ -2954,11 +2966,11 @@
       <c r="L18" s="30"/>
       <c r="M18" s="30">
         <f>IF($D18-SUM($E18:L18)&gt;M$5-SUM(M$7:M17),M$5-SUM(M$7:M17),$D18-SUM($E18:L18))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N18" s="30">
         <f>IF($D18-SUM($E18:M18)&gt;N$5-SUM(N$7:N17),N$5-SUM(N$7:N17),$D18-SUM($E18:M18))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O18" s="30">
         <f>IF($D18-SUM($E18:N18)&gt;O$5-SUM(O$7:O17),O$5-SUM(O$7:O17),$D18-SUM($E18:N18))</f>
@@ -2966,7 +2978,7 @@
       </c>
       <c r="P18" s="30">
         <f>IF($D18-SUM($E18:O18)&gt;P$5-SUM(P$7:P17),P$5-SUM(P$7:P17),$D18-SUM($E18:O18))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q18" s="30">
         <f>IF($D18-SUM($E18:P18)&gt;Q$5-SUM(Q$7:Q17),Q$5-SUM(Q$7:Q17),$D18-SUM($E18:P18))</f>
@@ -3024,11 +3036,11 @@
         <v>12</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C19" s="21"/>
       <c r="D19" s="64">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E19" s="26"/>
       <c r="F19" s="30">
@@ -3059,7 +3071,7 @@
       </c>
       <c r="N19" s="30">
         <f>IF($D19-SUM($E19:M19)&gt;N$5-SUM(N$7:N18),N$5-SUM(N$7:N18),$D19-SUM($E19:M19))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O19" s="30">
         <f>IF($D19-SUM($E19:N19)&gt;O$5-SUM(O$7:O18),O$5-SUM(O$7:O18),$D19-SUM($E19:N19))</f>
@@ -3067,7 +3079,7 @@
       </c>
       <c r="P19" s="30">
         <f>IF($D19-SUM($E19:O19)&gt;P$5-SUM(P$7:P18),P$5-SUM(P$7:P18),$D19-SUM($E19:O19))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q19" s="30">
         <f>IF($D19-SUM($E19:P19)&gt;Q$5-SUM(Q$7:Q18),Q$5-SUM(Q$7:Q18),$D19-SUM($E19:P19))</f>
@@ -3125,11 +3137,11 @@
         <v>13</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C20" s="22"/>
       <c r="D20" s="64">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E20" s="26"/>
       <c r="F20" s="30">
@@ -3160,25 +3172,25 @@
       </c>
       <c r="N20" s="30">
         <f>IF($D20-SUM($E20:M20)&gt;N$5-SUM(N$7:N19),N$5-SUM(N$7:N19),$D20-SUM($E20:M20))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O20" s="30">
         <f>IF($D20-SUM($E20:N20)&gt;O$5-SUM(O$7:O19),O$5-SUM(O$7:O19),$D20-SUM($E20:N20))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="P20" s="30">
         <f>IF($D20-SUM($E20:O20)&gt;P$5-SUM(P$7:P19),P$5-SUM(P$7:P19),$D20-SUM($E20:O20))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q20" s="30">
         <f>IF($D20-SUM($E20:P20)&gt;Q$5-SUM(Q$7:Q19),Q$5-SUM(Q$7:Q19),$D20-SUM($E20:P20))</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="R20" s="30"/>
       <c r="S20" s="30"/>
       <c r="T20" s="30">
         <f>IF($D20-SUM($E20:S20)&gt;T$5-SUM(T$7:T19),T$5-SUM(T$7:T19),$D20-SUM($E20:S20))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U20" s="30">
         <f>IF($D20-SUM($E20:T20)&gt;U$5-SUM(U$7:U19),U$5-SUM(U$7:U19),$D20-SUM($E20:T20))</f>
@@ -3226,11 +3238,11 @@
         <v>14</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C21" s="21"/>
       <c r="D21" s="64">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="E21" s="26"/>
       <c r="F21" s="30">
@@ -3265,7 +3277,7 @@
       </c>
       <c r="O21" s="30">
         <f>IF($D21-SUM($E21:N21)&gt;O$5-SUM(O$7:O20),O$5-SUM(O$7:O20),$D21-SUM($E21:N21))</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="P21" s="30">
         <f>IF($D21-SUM($E21:O21)&gt;P$5-SUM(P$7:P20),P$5-SUM(P$7:P20),$D21-SUM($E21:O21))</f>
@@ -3279,7 +3291,7 @@
       <c r="S21" s="30"/>
       <c r="T21" s="30">
         <f>IF($D21-SUM($E21:S21)&gt;T$5-SUM(T$7:T20),T$5-SUM(T$7:T20),$D21-SUM($E21:S21))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U21" s="30">
         <f>IF($D21-SUM($E21:T21)&gt;U$5-SUM(U$7:U20),U$5-SUM(U$7:U20),$D21-SUM($E21:T21))</f>
@@ -3326,9 +3338,13 @@
       <c r="A22" s="51">
         <v>15</v>
       </c>
-      <c r="B22" s="20"/>
+      <c r="B22" s="20" t="s">
+        <v>28</v>
+      </c>
       <c r="C22" s="21"/>
-      <c r="D22" s="64"/>
+      <c r="D22" s="64">
+        <v>4</v>
+      </c>
       <c r="E22" s="26"/>
       <c r="F22" s="30">
         <f>IF($D22-SUM($E22:E22)&gt;F$5-SUM(F$7:F21),F$5-SUM(F$7:F21),$D22-SUM($E22:E22))</f>
@@ -3362,11 +3378,11 @@
       </c>
       <c r="O22" s="30">
         <f>IF($D22-SUM($E22:N22)&gt;O$5-SUM(O$7:O21),O$5-SUM(O$7:O21),$D22-SUM($E22:N22))</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="P22" s="30">
         <f>IF($D22-SUM($E22:O22)&gt;P$5-SUM(P$7:P21),P$5-SUM(P$7:P21),$D22-SUM($E22:O22))</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="Q22" s="30">
         <f>IF($D22-SUM($E22:P22)&gt;Q$5-SUM(Q$7:Q21),Q$5-SUM(Q$7:Q21),$D22-SUM($E22:P22))</f>
@@ -3423,9 +3439,13 @@
       <c r="A23" s="51">
         <v>16</v>
       </c>
-      <c r="B23" s="20"/>
+      <c r="B23" s="20" t="s">
+        <v>29</v>
+      </c>
       <c r="C23" s="21"/>
-      <c r="D23" s="64"/>
+      <c r="D23" s="64">
+        <v>5</v>
+      </c>
       <c r="E23" s="26"/>
       <c r="F23" s="30">
         <f>IF($D23-SUM($E23:E23)&gt;F$5-SUM(F$7:F22),F$5-SUM(F$7:F22),$D23-SUM($E23:E23))</f>
@@ -3463,11 +3483,11 @@
       </c>
       <c r="P23" s="30">
         <f>IF($D23-SUM($E23:O23)&gt;P$5-SUM(P$7:P22),P$5-SUM(P$7:P22),$D23-SUM($E23:O23))</f>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="Q23" s="30">
         <f>IF($D23-SUM($E23:P23)&gt;Q$5-SUM(Q$7:Q22),Q$5-SUM(Q$7:Q22),$D23-SUM($E23:P23))</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="R23" s="30"/>
       <c r="S23" s="30"/>
@@ -3520,9 +3540,13 @@
       <c r="A24" s="51">
         <v>17</v>
       </c>
-      <c r="B24" s="20"/>
+      <c r="B24" s="20" t="s">
+        <v>30</v>
+      </c>
       <c r="C24" s="21"/>
-      <c r="D24" s="64"/>
+      <c r="D24" s="64">
+        <v>10</v>
+      </c>
       <c r="E24" s="26"/>
       <c r="F24" s="30">
         <f>IF($D24-SUM($E24:E24)&gt;F$5-SUM(F$7:F23),F$5-SUM(F$7:F23),$D24-SUM($E24:E24))</f>
@@ -3564,13 +3588,13 @@
       </c>
       <c r="Q24" s="30">
         <f>IF($D24-SUM($E24:P24)&gt;Q$5-SUM(Q$7:Q23),Q$5-SUM(Q$7:Q23),$D24-SUM($E24:P24))</f>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="R24" s="30"/>
       <c r="S24" s="30"/>
       <c r="T24" s="30">
         <f>IF($D24-SUM($E24:S24)&gt;T$5-SUM(T$7:T23),T$5-SUM(T$7:T23),$D24-SUM($E24:S24))</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="U24" s="30">
         <f>IF($D24-SUM($E24:T24)&gt;U$5-SUM(U$7:U23),U$5-SUM(U$7:U23),$D24-SUM($E24:T24))</f>
@@ -3617,9 +3641,13 @@
       <c r="A25" s="51">
         <v>18</v>
       </c>
-      <c r="B25" s="20"/>
+      <c r="B25" s="20" t="s">
+        <v>31</v>
+      </c>
       <c r="C25" s="21"/>
-      <c r="D25" s="64"/>
+      <c r="D25" s="64">
+        <v>5.5</v>
+      </c>
       <c r="E25" s="26"/>
       <c r="F25" s="30">
         <f>IF($D25-SUM($E25:E25)&gt;F$5-SUM(F$7:F24),F$5-SUM(F$7:F24),$D25-SUM($E25:E25))</f>
@@ -3667,7 +3695,7 @@
       <c r="S25" s="30"/>
       <c r="T25" s="30">
         <f>IF($D25-SUM($E25:S25)&gt;T$5-SUM(T$7:T24),T$5-SUM(T$7:T24),$D25-SUM($E25:S25))</f>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="U25" s="30">
         <f>IF($D25-SUM($E25:T25)&gt;U$5-SUM(U$7:U24),U$5-SUM(U$7:U24),$D25-SUM($E25:T25))</f>
@@ -11810,12 +11838,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <jeb5123c558143d5ab1e1526e87a8da0 xmlns="b7e4e9fd-5e36-4299-889f-f6136aff670e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </jeb5123c558143d5ab1e1526e87a8da0>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b7e4e9fd-5e36-4299-889f-f6136aff670e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Cohort xmlns="b7e4e9fd-5e36-4299-889f-f6136aff670e" xsi:nil="true"/>
+    <TaxCatchAll xmlns="fbafb59e-d651-4668-8e65-f7f85ceca18b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12108,26 +12144,28 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <jeb5123c558143d5ab1e1526e87a8da0 xmlns="b7e4e9fd-5e36-4299-889f-f6136aff670e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </jeb5123c558143d5ab1e1526e87a8da0>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b7e4e9fd-5e36-4299-889f-f6136aff670e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Cohort xmlns="b7e4e9fd-5e36-4299-889f-f6136aff670e" xsi:nil="true"/>
-    <TaxCatchAll xmlns="fbafb59e-d651-4668-8e65-f7f85ceca18b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E69471D0-9E76-49CC-83BD-A0DADDC861F7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C73059C-C1E8-4277-A8B4-81AF0BAF2A41}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b7e4e9fd-5e36-4299-889f-f6136aff670e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fbafb59e-d651-4668-8e65-f7f85ceca18b"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -12153,19 +12191,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C73059C-C1E8-4277-A8B4-81AF0BAF2A41}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E69471D0-9E76-49CC-83BD-A0DADDC861F7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b7e4e9fd-5e36-4299-889f-f6136aff670e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fbafb59e-d651-4668-8e65-f7f85ceca18b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>